<commit_message>
Trade update - 2026-02-19 22:22 UTC
</commit_message>
<xml_diff>
--- a/trade_tracker.xlsx
+++ b/trade_tracker.xlsx
@@ -19,9 +19,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="$#,##0.0000;-$#,##0.0000"/>
-    <numFmt numFmtId="165" formatCode="₹#,##0.00;-₹#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="$#,##0.0000;-$#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="₹#,##0.00;-₹#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -97,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -105,19 +105,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -657,16 +669,16 @@
           <t>03:30</t>
         </is>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="8" t="n">
         <v>66447.89999999999</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="8" t="n">
         <v>66400</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="8" t="n">
         <v>68800</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="8" t="n">
         <v>61000</v>
       </c>
       <c r="I2" s="2" t="n">
@@ -675,28 +687,28 @@
       <c r="J2" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="K2" s="3" t="n">
+      <c r="K2" s="8" t="n">
         <v>65</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="n">
+      <c r="M2" s="8" t="n">
         <v>75</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="N2" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P2" s="3" t="n">
+      <c r="P2" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="Q2" s="4" t="n">
+      <c r="Q2" s="9" t="n">
         <v>59</v>
       </c>
-      <c r="R2" s="5" t="n">
+      <c r="R2" s="10" t="n">
         <v>5355.43</v>
       </c>
       <c r="S2" s="6" t="n">
@@ -717,8 +729,94 @@
           <t>DRY RUN</t>
         </is>
       </c>
-      <c r="W2" s="7">
+      <c r="W2" s="11">
         <f>R2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>19-02-2026</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>03:52</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>66447.89999999999</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>66400</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>68800</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>61000</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8" t="n">
+        <v>65</v>
+      </c>
+      <c r="L3" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="N3" s="8" t="n">
+        <v>18</v>
+      </c>
+      <c r="O3" s="8" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P3" s="8" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="Q3" s="9" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="R3" s="10" t="n">
+        <v>5046.81</v>
+      </c>
+      <c r="S3" s="6" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>Time Exit (5:15 PM)</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>0h 0m</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>DRY RUN</t>
+        </is>
+      </c>
+      <c r="W3" s="11">
+        <f>W2+R3</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
[EXIT] 2026-02-26 12:06 UTC
</commit_message>
<xml_diff>
--- a/trade_tracker.xlsx
+++ b/trade_tracker.xlsx
@@ -23,7 +23,7 @@
     <numFmt numFmtId="165" formatCode="$#,##0.0000;-$#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="₹#,##0.00;-₹#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -52,8 +52,14 @@
       <b val="1"/>
       <sz val="9"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="00006100"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -68,6 +74,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,6 +129,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -722,6 +742,92 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>26-02-2026</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>03:53</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>68888.5</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>68800</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>70800</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>66600</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>167</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8" t="n">
+        <v>167</v>
+      </c>
+      <c r="R3" s="9" t="n">
+        <v>15190.32</v>
+      </c>
+      <c r="S3" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>Time Exit — Options Expired OTM (full premium kept)</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>13h 43m</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>DRY RUN</t>
+        </is>
+      </c>
+      <c r="W3" s="7">
+        <f>W2+R3</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:W1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[EXIT] 2026-03-01 11:51 UTC
</commit_message>
<xml_diff>
--- a/trade_tracker.xlsx
+++ b/trade_tracker.xlsx
@@ -23,7 +23,7 @@
     <numFmt numFmtId="165" formatCode="$#,##0.0000;-$#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="₹#,##0.00;-₹#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -52,8 +52,14 @@
       <b val="1"/>
       <sz val="9"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="009C0006"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -68,6 +74,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,6 +129,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -722,6 +742,92 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>01-03-2026</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>03:44</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>07:55</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>66890</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>66800</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>70400</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>64000</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>27.75</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>52.75</v>
+      </c>
+      <c r="Q3" s="8" t="n">
+        <v>-31.65</v>
+      </c>
+      <c r="R3" s="9" t="n">
+        <v>-2883.63</v>
+      </c>
+      <c r="S3" s="10" t="n">
+        <v>-150</v>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>SL — Combined 2.5x (intraday @ 07:55)</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr">
+        <is>
+          <t>4h 11m</t>
+        </is>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>DRY RUN</t>
+        </is>
+      </c>
+      <c r="W3" s="7">
+        <f>W2+R3</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:W1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>